<commit_message>
updated enigma combat with motor scores
</commit_message>
<xml_diff>
--- a/cortical_atrophy/data/FREESURFER_ENIGMA/QCtable_distance_voxels_manualQC.xlsx
+++ b/cortical_atrophy/data/FREESURFER_ENIGMA/QCtable_distance_voxels_manualQC.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilyolafson/GIT/ENIGMA/enigma_disconnections/cortical_atrophy/data/FREESURFER_ENIGMA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A1D33272-6AEA-9341-86E0-A92B5E408B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CE04A5E2-4BCB-3348-8F25-1275E8E41443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="820" windowWidth="23260" windowHeight="24300"/>
+    <workbookView xWindow="160" yWindow="3260" windowWidth="23260" windowHeight="24300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QCtable_distance_voxels_manualQ" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,48 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={D4EFAA5D-E9F5-8246-BE53-A4FB2526A124}</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="1025" xr:uid="{D4EFAA5D-E9F5-8246-BE53-A4FB2526A124}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    QC done in MNI space..
+</t>
+      </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor>
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>190500</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>25400</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>685800</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>88900</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1151" uniqueCount="1113">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1182" uniqueCount="1134">
   <si>
     <t>Subject</t>
   </si>
@@ -3364,12 +3404,75 @@
   </si>
   <si>
     <t>small failure rh temporal ctx, small failures intersecting with the lesion</t>
+  </si>
+  <si>
+    <t>crazy ventricles, distortion</t>
+  </si>
+  <si>
+    <t>medium failures lh and rh temporal ctx, failure to segment rh frontal lobe past lesion</t>
+  </si>
+  <si>
+    <t>small failure rh and lh temporal ctx, some cortical undersegmentation superior/frontal as well</t>
+  </si>
+  <si>
+    <t>failures intersecting with the lesion</t>
+  </si>
+  <si>
+    <t>small failures lh and rh temporal ctx</t>
+  </si>
+  <si>
+    <t>severely undersegmented rh parietal area but intersecting w lesion and otherwise ok?</t>
+  </si>
+  <si>
+    <t>registration failure/bad distortion</t>
+  </si>
+  <si>
+    <t>weird disrortion around temporal poles</t>
+  </si>
+  <si>
+    <t>distortion and lots of undersegmentation superior parietal</t>
+  </si>
+  <si>
+    <t>pretty big failure parietal ctx rh due to lesion (and parts of lh too)</t>
+  </si>
+  <si>
+    <t>random freesurfer failure to properly segment many cortical &amp; cerebellar regions]</t>
+  </si>
+  <si>
+    <t>unique temporal lobe failure (distortion?) and underseg superior ctx</t>
+  </si>
+  <si>
+    <t>lh inferior frontal ctx undersegmentation. Weirdness around insula</t>
+  </si>
+  <si>
+    <t>weird registration? Distortion</t>
+  </si>
+  <si>
+    <t>weird registration</t>
+  </si>
+  <si>
+    <t>light undersegmentation rh and lh temporal ctx</t>
+  </si>
+  <si>
+    <t>double check registration</t>
+  </si>
+  <si>
+    <t>check registration</t>
+  </si>
+  <si>
+    <t>big lesion. lots of failure intersecting w the lesion. Contralesional is probably best here.</t>
+  </si>
+  <si>
+    <t>rh insula underseg and temporal pole. Also pretty bad superior frontal underseg lh and rh girl!</t>
+  </si>
+  <si>
+    <t>moderate failure superior parietal ctx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3914,6 +4017,86 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor editAs="absolute">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>190500</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>685800</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Comment 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A69CEF5-280A-3BFF-30C7-5AEC44D5B9FA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="6032500" y="25400"/>
+              <a:ext cx="1320800" cy="876300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFE1" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="80"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="510000"/>
+              </a:solidFill>
+              <a:miter lim="800%"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://purl.oclc.org/ooxml/spreadsheetml/main">
+  <person displayName="Emily Olafson" id="{6538935B-6BBA-9E4B-A209-3C693317D527}" userId="S::emo4002@med.cornell.edu::0d859566-d533-4f5a-9367-0f125312e4fd" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
@@ -4209,12 +4392,21 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://purl.oclc.org/ooxml/spreadsheetml/main">
+  <threadedComment ref="E1" dT="2022-10-17T18:34:45.50" personId="{6538935B-6BBA-9E4B-A209-3C693317D527}" id="{D4EFAA5D-E9F5-8246-BE53-A4FB2526A124}">
+    <text xml:space="preserve">QC done in MNI space..
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1069"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="E170" sqref="E170"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="F219" sqref="F219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7295,6 +7487,9 @@
       <c r="D170">
         <v>1</v>
       </c>
+      <c r="E170">
+        <v>1</v>
+      </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171">
@@ -7309,6 +7504,9 @@
       <c r="D171">
         <v>1</v>
       </c>
+      <c r="E171">
+        <v>1</v>
+      </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172">
@@ -7323,6 +7521,12 @@
       <c r="D172">
         <v>1</v>
       </c>
+      <c r="E172">
+        <v>0</v>
+      </c>
+      <c r="F172" t="s">
+        <v>1113</v>
+      </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173">
@@ -7337,6 +7541,9 @@
       <c r="D173">
         <v>1</v>
       </c>
+      <c r="E173">
+        <v>1</v>
+      </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174">
@@ -7351,6 +7558,9 @@
       <c r="D174">
         <v>1</v>
       </c>
+      <c r="E174">
+        <v>1</v>
+      </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175">
@@ -7365,6 +7575,12 @@
       <c r="D175">
         <v>1</v>
       </c>
+      <c r="E175">
+        <v>0</v>
+      </c>
+      <c r="F175" t="s">
+        <v>1114</v>
+      </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176">
@@ -7379,8 +7595,11 @@
       <c r="D176">
         <v>1</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>175</v>
       </c>
@@ -7393,8 +7612,14 @@
       <c r="D177">
         <v>1</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E177">
+        <v>0.5</v>
+      </c>
+      <c r="F177" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>176</v>
       </c>
@@ -7407,8 +7632,11 @@
       <c r="D178">
         <v>1</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>177</v>
       </c>
@@ -7421,8 +7649,14 @@
       <c r="D179">
         <v>1</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E179">
+        <v>1</v>
+      </c>
+      <c r="F179" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>178</v>
       </c>
@@ -7435,8 +7669,14 @@
       <c r="D180">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E180">
+        <v>0</v>
+      </c>
+      <c r="F180" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>179</v>
       </c>
@@ -7449,8 +7689,14 @@
       <c r="D181">
         <v>1</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E181">
+        <v>0.5</v>
+      </c>
+      <c r="F181" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>180</v>
       </c>
@@ -7463,8 +7709,14 @@
       <c r="D182">
         <v>1</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E182">
+        <v>0.5</v>
+      </c>
+      <c r="F182" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>181</v>
       </c>
@@ -7477,8 +7729,14 @@
       <c r="D183">
         <v>1</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>182</v>
       </c>
@@ -7491,8 +7749,11 @@
       <c r="D184">
         <v>1</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>183</v>
       </c>
@@ -7505,8 +7766,14 @@
       <c r="D185">
         <v>1</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E185">
+        <v>0.5</v>
+      </c>
+      <c r="F185" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>184</v>
       </c>
@@ -7519,8 +7786,14 @@
       <c r="D186">
         <v>1</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E186">
+        <v>0.5</v>
+      </c>
+      <c r="F186" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>185</v>
       </c>
@@ -7533,8 +7806,14 @@
       <c r="D187">
         <v>1</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E187">
+        <v>0.5</v>
+      </c>
+      <c r="F187" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>186</v>
       </c>
@@ -7547,8 +7826,14 @@
       <c r="D188">
         <v>1</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E188">
+        <v>1</v>
+      </c>
+      <c r="F188" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>187</v>
       </c>
@@ -7561,8 +7846,11 @@
       <c r="D189">
         <v>1</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>188</v>
       </c>
@@ -7575,8 +7863,14 @@
       <c r="D190">
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E190">
+        <v>1</v>
+      </c>
+      <c r="F190" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>189</v>
       </c>
@@ -7589,8 +7883,14 @@
       <c r="D191">
         <v>1</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E191">
+        <v>0</v>
+      </c>
+      <c r="F191" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>190</v>
       </c>
@@ -7603,8 +7903,14 @@
       <c r="D192">
         <v>1</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E192">
+        <v>1</v>
+      </c>
+      <c r="F192" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>191</v>
       </c>
@@ -7617,8 +7923,14 @@
       <c r="D193">
         <v>1</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E193">
+        <v>1</v>
+      </c>
+      <c r="F193" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>192</v>
       </c>
@@ -7631,8 +7943,14 @@
       <c r="D194">
         <v>1</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E194">
+        <v>1</v>
+      </c>
+      <c r="F194" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>193</v>
       </c>
@@ -7645,8 +7963,14 @@
       <c r="D195">
         <v>1</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E195">
+        <v>1</v>
+      </c>
+      <c r="F195" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>194</v>
       </c>
@@ -7659,8 +7983,14 @@
       <c r="D196">
         <v>1</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E196">
+        <v>0</v>
+      </c>
+      <c r="F196" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>195</v>
       </c>
@@ -7673,8 +8003,14 @@
       <c r="D197">
         <v>1</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E197">
+        <v>0</v>
+      </c>
+      <c r="F197" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>196</v>
       </c>
@@ -7687,8 +8023,14 @@
       <c r="D198">
         <v>1</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E198">
+        <v>0.5</v>
+      </c>
+      <c r="F198" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>197</v>
       </c>
@@ -7701,8 +8043,14 @@
       <c r="D199">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E199">
+        <v>0.5</v>
+      </c>
+      <c r="F199" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>198</v>
       </c>
@@ -7715,8 +8063,11 @@
       <c r="D200">
         <v>1</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>199</v>
       </c>
@@ -7729,8 +8080,11 @@
       <c r="D201">
         <v>1</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>200</v>
       </c>
@@ -7743,8 +8097,14 @@
       <c r="D202">
         <v>1</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E202">
+        <v>0</v>
+      </c>
+      <c r="F202" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>201</v>
       </c>
@@ -7757,8 +8117,11 @@
       <c r="D203">
         <v>1</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>202</v>
       </c>
@@ -7771,8 +8134,14 @@
       <c r="D204">
         <v>1</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E204">
+        <v>0.5</v>
+      </c>
+      <c r="F204" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>203</v>
       </c>
@@ -7785,8 +8154,11 @@
       <c r="D205">
         <v>1</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>204</v>
       </c>
@@ -7799,8 +8171,14 @@
       <c r="D206">
         <v>1</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E206">
+        <v>0.5</v>
+      </c>
+      <c r="F206" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>205</v>
       </c>
@@ -7808,7 +8186,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>206</v>
       </c>
@@ -7821,8 +8199,14 @@
       <c r="D208">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E208">
+        <v>1</v>
+      </c>
+      <c r="F208" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>207</v>
       </c>
@@ -7835,8 +8219,11 @@
       <c r="D209">
         <v>1</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>208</v>
       </c>
@@ -7849,8 +8236,14 @@
       <c r="D210">
         <v>1</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E210">
+        <v>0</v>
+      </c>
+      <c r="F210" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>209</v>
       </c>
@@ -7863,8 +8256,11 @@
       <c r="D211">
         <v>1</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>210</v>
       </c>
@@ -7877,8 +8273,14 @@
       <c r="D212">
         <v>1</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E212">
+        <v>0</v>
+      </c>
+      <c r="F212" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>211</v>
       </c>
@@ -7891,8 +8293,14 @@
       <c r="D213">
         <v>1</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E213">
+        <v>0</v>
+      </c>
+      <c r="F213" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>212</v>
       </c>
@@ -7905,8 +8313,11 @@
       <c r="D214">
         <v>1</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>213</v>
       </c>
@@ -7919,8 +8330,11 @@
       <c r="D215">
         <v>1</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>214</v>
       </c>
@@ -7933,8 +8347,14 @@
       <c r="D216">
         <v>1</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E216">
+        <v>0.5</v>
+      </c>
+      <c r="F216" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>215</v>
       </c>
@@ -7947,8 +8367,11 @@
       <c r="D217">
         <v>1</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>216</v>
       </c>
@@ -7961,8 +8384,14 @@
       <c r="D218">
         <v>1</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E218">
+        <v>0.5</v>
+      </c>
+      <c r="F218" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>217</v>
       </c>
@@ -7976,7 +8405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>218</v>
       </c>
@@ -7990,7 +8419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>219</v>
       </c>
@@ -8004,7 +8433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>220</v>
       </c>
@@ -8018,7 +8447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>221</v>
       </c>
@@ -8032,7 +8461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>222</v>
       </c>
@@ -19224,5 +19653,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="v">
+      <legacyDrawing r:id="rId2"/>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>